<commit_message>
Corecciones de estatutos ciclicos y write
</commit_message>
<xml_diff>
--- a/docs/matriz-tokens.xlsx
+++ b/docs/matriz-tokens.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lexico" sheetId="1" r:id="rId1"/>
@@ -476,7 +476,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -503,6 +503,7 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -870,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -3219,10 +3220,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP45"/>
+  <dimension ref="A1:AP46"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -6812,7 +6813,7 @@
         <v>600</v>
       </c>
       <c r="Z38" s="24">
-        <v>33</v>
+        <v>600</v>
       </c>
       <c r="AA38" s="24">
         <v>600</v>
@@ -6892,7 +6893,7 @@
         <v>600</v>
       </c>
       <c r="V39" s="24">
-        <v>600</v>
+        <v>36</v>
       </c>
       <c r="W39" s="24">
         <v>600</v>
@@ -6904,7 +6905,7 @@
         <v>12</v>
       </c>
       <c r="Z39" s="24">
-        <v>600</v>
+        <v>33</v>
       </c>
       <c r="AA39" s="24">
         <v>600</v>
@@ -6993,7 +6994,7 @@
         <v>600</v>
       </c>
       <c r="Y40" s="24">
-        <v>600</v>
+        <v>12</v>
       </c>
       <c r="Z40" s="24">
         <v>600</v>
@@ -7011,9 +7012,106 @@
         <v>600</v>
       </c>
     </row>
-    <row r="45" spans="1:31">
-      <c r="AC45" s="9"/>
-      <c r="AD45" s="9"/>
+    <row r="41" spans="1:31">
+      <c r="A41" s="10">
+        <v>37</v>
+      </c>
+      <c r="B41" s="24">
+        <v>600</v>
+      </c>
+      <c r="C41" s="24">
+        <v>600</v>
+      </c>
+      <c r="D41" s="24">
+        <v>600</v>
+      </c>
+      <c r="E41" s="24">
+        <v>600</v>
+      </c>
+      <c r="F41" s="24">
+        <v>600</v>
+      </c>
+      <c r="G41" s="24">
+        <v>600</v>
+      </c>
+      <c r="H41" s="24">
+        <v>600</v>
+      </c>
+      <c r="I41" s="24">
+        <v>600</v>
+      </c>
+      <c r="J41" s="24">
+        <v>600</v>
+      </c>
+      <c r="K41" s="24">
+        <v>600</v>
+      </c>
+      <c r="L41" s="24">
+        <v>600</v>
+      </c>
+      <c r="M41" s="24">
+        <v>600</v>
+      </c>
+      <c r="N41" s="24">
+        <v>600</v>
+      </c>
+      <c r="O41" s="24">
+        <v>600</v>
+      </c>
+      <c r="P41" s="24">
+        <v>600</v>
+      </c>
+      <c r="Q41" s="24">
+        <v>600</v>
+      </c>
+      <c r="R41" s="24">
+        <v>600</v>
+      </c>
+      <c r="S41" s="24">
+        <v>600</v>
+      </c>
+      <c r="T41" s="24">
+        <v>600</v>
+      </c>
+      <c r="U41" s="24">
+        <v>600</v>
+      </c>
+      <c r="V41" s="24">
+        <v>600</v>
+      </c>
+      <c r="W41" s="24">
+        <v>600</v>
+      </c>
+      <c r="X41" s="24">
+        <v>600</v>
+      </c>
+      <c r="Y41" s="24">
+        <v>600</v>
+      </c>
+      <c r="Z41" s="24">
+        <v>600</v>
+      </c>
+      <c r="AA41" s="24">
+        <v>600</v>
+      </c>
+      <c r="AB41" s="24">
+        <v>600</v>
+      </c>
+      <c r="AC41" s="24">
+        <v>600</v>
+      </c>
+      <c r="AD41" s="24">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31">
+      <c r="A42" s="26">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31">
+      <c r="AC46" s="9"/>
+      <c r="AD46" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7023,10 +7121,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE114"/>
+  <dimension ref="A1:AE115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -7038,593 +7136,648 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" s="6" t="s">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="W1">
+        <v>21</v>
+      </c>
+      <c r="X1">
+        <v>22</v>
+      </c>
+      <c r="Y1">
+        <v>23</v>
+      </c>
+      <c r="Z1">
+        <v>24</v>
+      </c>
+      <c r="AA1">
+        <v>25</v>
+      </c>
+      <c r="AB1">
+        <v>26</v>
+      </c>
+      <c r="AC1">
+        <v>27</v>
+      </c>
+      <c r="AD1">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:31">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="6"/>
-    </row>
-    <row r="2" spans="1:31">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7">
+      <c r="AE2" s="6"/>
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7">
         <v>100</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C3" s="6">
         <v>101</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D3" s="6">
         <v>102</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E3" s="6">
         <v>103</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F3" s="6">
         <v>104</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G3" s="6">
         <v>105</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H3" s="6">
         <v>106</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I3" s="6">
         <v>107</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J3" s="6">
         <v>108</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K3" s="6">
         <v>109</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L3" s="6">
         <v>110</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M3" s="6">
         <v>111</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N3" s="6">
         <v>112</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O3" s="6">
         <v>113</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P3" s="6">
         <v>114</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q3" s="6">
         <v>115</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R3" s="6">
         <v>116</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S3" s="6">
         <v>117</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T3" s="6">
         <v>118</v>
       </c>
-      <c r="U2" s="6">
+      <c r="U3" s="6">
         <v>119</v>
       </c>
-      <c r="V2" s="6">
+      <c r="V3" s="6">
         <v>120</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W3" s="6">
         <v>121</v>
       </c>
-      <c r="X2" s="6">
+      <c r="X3" s="6">
         <v>122</v>
       </c>
-      <c r="Y2" s="6">
+      <c r="Y3" s="6">
         <v>123</v>
       </c>
-      <c r="Z2" s="6">
+      <c r="Z3" s="6">
         <v>124</v>
       </c>
-      <c r="AA2" s="6">
+      <c r="AA3" s="6">
         <v>125</v>
       </c>
-      <c r="AB2" s="6">
+      <c r="AB3" s="6">
         <v>126</v>
       </c>
-      <c r="AC2" s="6">
+      <c r="AC3" s="6">
         <v>127</v>
       </c>
-      <c r="AD2" s="6">
+      <c r="AD3" s="6">
         <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>600</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>600</v>
-      </c>
-      <c r="H3">
-        <v>600</v>
-      </c>
-      <c r="I3">
-        <v>600</v>
-      </c>
-      <c r="J3">
-        <v>600</v>
-      </c>
-      <c r="K3">
-        <v>600</v>
-      </c>
-      <c r="L3">
-        <v>600</v>
-      </c>
-      <c r="M3">
-        <v>600</v>
-      </c>
-      <c r="N3">
-        <v>600</v>
-      </c>
-      <c r="O3">
-        <v>600</v>
-      </c>
-      <c r="P3">
-        <v>600</v>
-      </c>
-      <c r="Q3">
-        <v>600</v>
-      </c>
-      <c r="R3">
-        <v>2</v>
-      </c>
-      <c r="S3">
-        <v>600</v>
-      </c>
-      <c r="T3">
-        <v>600</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>600</v>
-      </c>
-      <c r="X3">
-        <v>400</v>
-      </c>
-      <c r="Y3">
-        <v>600</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>1</v>
-      </c>
-      <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AC3">
-        <v>600</v>
-      </c>
-      <c r="AD3">
-        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:31">
       <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>600</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>400</v>
-      </c>
-      <c r="C4">
-        <v>400</v>
-      </c>
-      <c r="D4">
-        <v>400</v>
-      </c>
       <c r="E4">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="G4">
+        <v>600</v>
+      </c>
+      <c r="H4">
+        <v>600</v>
+      </c>
+      <c r="I4">
+        <v>600</v>
+      </c>
+      <c r="J4">
+        <v>600</v>
+      </c>
+      <c r="K4">
+        <v>600</v>
+      </c>
+      <c r="L4">
+        <v>600</v>
+      </c>
+      <c r="M4">
+        <v>600</v>
+      </c>
+      <c r="N4">
+        <v>600</v>
+      </c>
+      <c r="O4">
+        <v>600</v>
+      </c>
+      <c r="P4">
+        <v>600</v>
+      </c>
+      <c r="Q4">
+        <v>600</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>600</v>
+      </c>
+      <c r="T4">
+        <v>600</v>
+      </c>
+      <c r="U4">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="V4">
         <v>0</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>400</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>400</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>400</v>
-      </c>
-      <c r="V4">
-        <v>400</v>
-      </c>
       <c r="W4">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="X4">
         <v>400</v>
       </c>
       <c r="Y4">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="Z4">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="AB4">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="AC4">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="AD4">
-        <v>400</v>
+        <v>600</v>
       </c>
     </row>
     <row r="5" spans="1:31">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="C5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="G5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="L5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="S5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="V5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="W5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="X5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="Y5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="Z5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="AA5">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="AB5">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="AC5">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="AD5">
-        <v>600</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:31">
       <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>600</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>600</v>
+      </c>
+      <c r="H6">
+        <v>600</v>
+      </c>
+      <c r="I6">
+        <v>600</v>
+      </c>
+      <c r="J6">
+        <v>600</v>
+      </c>
+      <c r="K6">
+        <v>600</v>
+      </c>
+      <c r="L6">
+        <v>600</v>
+      </c>
+      <c r="M6">
+        <v>600</v>
+      </c>
+      <c r="N6">
+        <v>600</v>
+      </c>
+      <c r="O6">
+        <v>600</v>
+      </c>
+      <c r="P6">
+        <v>600</v>
+      </c>
+      <c r="Q6">
+        <v>600</v>
+      </c>
+      <c r="R6">
+        <v>600</v>
+      </c>
+      <c r="S6">
+        <v>600</v>
+      </c>
+      <c r="T6">
+        <v>600</v>
+      </c>
+      <c r="U6">
+        <v>600</v>
+      </c>
+      <c r="V6">
+        <v>600</v>
+      </c>
+      <c r="W6">
+        <v>600</v>
+      </c>
+      <c r="X6">
+        <v>600</v>
+      </c>
+      <c r="Y6">
+        <v>600</v>
+      </c>
+      <c r="Z6">
+        <v>600</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>600</v>
+      </c>
+      <c r="AD6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>400</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>400</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>400</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>400</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>400</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <v>0</v>
       </c>
-      <c r="K6">
+      <c r="K7">
         <v>400</v>
       </c>
-      <c r="L6">
+      <c r="L7">
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="M7">
         <v>0</v>
       </c>
-      <c r="N6">
+      <c r="N7">
         <v>0</v>
       </c>
-      <c r="O6">
+      <c r="O7">
         <v>0</v>
       </c>
-      <c r="P6">
+      <c r="P7">
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="Q7">
         <v>0</v>
       </c>
-      <c r="R6">
+      <c r="R7">
         <v>400</v>
       </c>
-      <c r="S6">
+      <c r="S7">
         <v>0</v>
       </c>
-      <c r="T6">
+      <c r="T7">
         <v>0</v>
       </c>
-      <c r="U6">
+      <c r="U7">
         <v>400</v>
       </c>
-      <c r="V6">
+      <c r="V7">
         <v>400</v>
       </c>
-      <c r="W6">
+      <c r="W7">
         <v>0</v>
       </c>
-      <c r="X6">
+      <c r="X7">
         <v>400</v>
       </c>
-      <c r="Y6">
+      <c r="Y7">
         <v>400</v>
       </c>
-      <c r="Z6">
+      <c r="Z7">
         <v>400</v>
       </c>
-      <c r="AA6">
+      <c r="AA7">
         <v>400</v>
       </c>
-      <c r="AB6">
+      <c r="AB7">
         <v>400</v>
       </c>
-      <c r="AC6">
+      <c r="AC7">
         <v>400</v>
       </c>
-      <c r="AD6">
+      <c r="AD7">
         <v>400</v>
       </c>
-    </row>
-    <row r="7" spans="1:31">
-      <c r="A7" s="8">
-        <v>4</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="8"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="8"/>
     </row>
     <row r="8" spans="1:31">
       <c r="A8" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -7658,7 +7811,7 @@
     </row>
     <row r="9" spans="1:31">
       <c r="A9" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -7692,7 +7845,7 @@
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -7726,7 +7879,7 @@
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -7755,12 +7908,12 @@
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
       <c r="AB11" s="8"/>
-      <c r="AC11" s="14"/>
+      <c r="AC11" s="8"/>
       <c r="AD11" s="8"/>
     </row>
     <row r="12" spans="1:31">
       <c r="A12" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -7789,12 +7942,12 @@
       <c r="Z12" s="8"/>
       <c r="AA12" s="8"/>
       <c r="AB12" s="8"/>
-      <c r="AC12" s="8"/>
+      <c r="AC12" s="14"/>
       <c r="AD12" s="8"/>
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -7828,7 +7981,7 @@
     </row>
     <row r="14" spans="1:31">
       <c r="A14" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -7862,7 +8015,7 @@
     </row>
     <row r="15" spans="1:31">
       <c r="A15" s="8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -7896,7 +8049,7 @@
     </row>
     <row r="16" spans="1:31">
       <c r="A16" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -7930,7 +8083,7 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="8">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -7964,7 +8117,7 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -7998,7 +8151,7 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -8031,477 +8184,511 @@
       <c r="AD19" s="8"/>
     </row>
     <row r="20" spans="1:30">
-      <c r="A20">
-        <v>17</v>
-      </c>
+      <c r="A20" s="8">
+        <v>16</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
     </row>
     <row r="21" spans="1:30">
       <c r="A21">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:30">
       <c r="A22">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:30">
       <c r="A23">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:30">
       <c r="A24">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:30">
       <c r="A25">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:30">
       <c r="A26">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:30">
       <c r="A27">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:30">
       <c r="A28">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:30">
       <c r="A29">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:30">
       <c r="A30">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:30">
       <c r="A31">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:30">
       <c r="A32">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Acciones semanticas de declaracion
Creacion de la tabla de simbolos
</commit_message>
<xml_diff>
--- a/docs/matriz-tokens.xlsx
+++ b/docs/matriz-tokens.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Sintactico" sheetId="3" r:id="rId2"/>
     <sheet name="expresion" sheetId="6" r:id="rId3"/>
     <sheet name="Hoja1" sheetId="9" r:id="rId4"/>
+    <sheet name="Hoja2" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="88">
   <si>
     <t>l</t>
   </si>
@@ -266,6 +267,21 @@
   </si>
   <si>
     <t>37)endclass</t>
+  </si>
+  <si>
+    <t>edo</t>
+  </si>
+  <si>
+    <t>accion semantica</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>Agrega un identificador a la tabla de simbolos</t>
+  </si>
+  <si>
+    <t>Agrega tipo en ap, incrementa apuntador en 1</t>
   </si>
 </sst>
 </file>
@@ -3225,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -8769,4 +8785,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>900</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>901</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corregi matriz de producciones
Les habia puesto coma al final de cada produccion y era punto y coma, ya
lo solucione, el archivo sigue estando en la carpeta docs
</commit_message>
<xml_diff>
--- a/docs/matriz-tokens.xlsx
+++ b/docs/matriz-tokens.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose\Documents\GitHub\compiler-intepreter\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
@@ -501,8 +506,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -842,6 +847,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1215,14 +1228,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5" style="34" bestFit="1" customWidth="1"/>
     <col min="2" max="247" width="11" style="33"/>
@@ -1480,7 +1493,7 @@
     <col min="16175" max="16384" width="11" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="30" customFormat="1" ht="69" customHeight="1">
+    <row r="1" spans="1:47" s="30" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>88</v>
       </c>
@@ -1623,7 +1636,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="24.75" customHeight="1">
+    <row r="2" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>98</v>
       </c>
@@ -1674,7 +1687,7 @@
       <c r="AT2" s="32"/>
       <c r="AU2" s="32"/>
     </row>
-    <row r="3" spans="1:47" ht="24.75" customHeight="1">
+    <row r="3" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>99</v>
       </c>
@@ -1725,7 +1738,7 @@
       <c r="AT3" s="32"/>
       <c r="AU3" s="32"/>
     </row>
-    <row r="4" spans="1:47" ht="24.75" customHeight="1">
+    <row r="4" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>100</v>
       </c>
@@ -1776,7 +1789,7 @@
       <c r="AT4" s="32"/>
       <c r="AU4" s="32"/>
     </row>
-    <row r="5" spans="1:47" ht="24.75" customHeight="1">
+    <row r="5" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>101</v>
       </c>
@@ -1827,7 +1840,7 @@
       <c r="AT5" s="32"/>
       <c r="AU5" s="32"/>
     </row>
-    <row r="6" spans="1:47" ht="24.75" customHeight="1">
+    <row r="6" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>102</v>
       </c>
@@ -1878,7 +1891,7 @@
       <c r="AT6" s="32"/>
       <c r="AU6" s="32"/>
     </row>
-    <row r="7" spans="1:47" ht="24.75" customHeight="1">
+    <row r="7" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>103</v>
       </c>
@@ -1929,7 +1942,7 @@
       <c r="AT7" s="32"/>
       <c r="AU7" s="32"/>
     </row>
-    <row r="8" spans="1:47" ht="24.75" customHeight="1">
+    <row r="8" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>104</v>
       </c>
@@ -1980,7 +1993,7 @@
       <c r="AT8" s="32"/>
       <c r="AU8" s="32"/>
     </row>
-    <row r="9" spans="1:47" ht="24.75" customHeight="1">
+    <row r="9" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>105</v>
       </c>
@@ -2031,7 +2044,7 @@
       <c r="AT9" s="32"/>
       <c r="AU9" s="32"/>
     </row>
-    <row r="10" spans="1:47" ht="24.75" customHeight="1">
+    <row r="10" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>106</v>
       </c>
@@ -2082,7 +2095,7 @@
       <c r="AT10" s="32"/>
       <c r="AU10" s="32"/>
     </row>
-    <row r="11" spans="1:47" ht="24.75" customHeight="1">
+    <row r="11" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>107</v>
       </c>
@@ -2133,7 +2146,7 @@
       <c r="AT11" s="32"/>
       <c r="AU11" s="32"/>
     </row>
-    <row r="12" spans="1:47" ht="24.75" customHeight="1">
+    <row r="12" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>108</v>
       </c>
@@ -2184,7 +2197,7 @@
       <c r="AT12" s="32"/>
       <c r="AU12" s="32"/>
     </row>
-    <row r="13" spans="1:47" ht="24.75" customHeight="1">
+    <row r="13" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>109</v>
       </c>
@@ -2235,7 +2248,7 @@
       <c r="AT13" s="32"/>
       <c r="AU13" s="32"/>
     </row>
-    <row r="14" spans="1:47" ht="24.75" customHeight="1">
+    <row r="14" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>110</v>
       </c>
@@ -2286,7 +2299,7 @@
       <c r="AT14" s="32"/>
       <c r="AU14" s="32"/>
     </row>
-    <row r="15" spans="1:47" ht="24.75" customHeight="1">
+    <row r="15" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>111</v>
       </c>
@@ -2337,7 +2350,7 @@
       <c r="AT15" s="32"/>
       <c r="AU15" s="32"/>
     </row>
-    <row r="16" spans="1:47" ht="24.75" customHeight="1">
+    <row r="16" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>112</v>
       </c>
@@ -2388,7 +2401,7 @@
       <c r="AT16" s="32"/>
       <c r="AU16" s="32"/>
     </row>
-    <row r="17" spans="1:47" ht="24.75" customHeight="1">
+    <row r="17" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>113</v>
       </c>
@@ -2439,7 +2452,7 @@
       <c r="AT17" s="32"/>
       <c r="AU17" s="32"/>
     </row>
-    <row r="18" spans="1:47" ht="24.75" customHeight="1">
+    <row r="18" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>114</v>
       </c>
@@ -2490,7 +2503,7 @@
       <c r="AT18" s="32"/>
       <c r="AU18" s="32"/>
     </row>
-    <row r="19" spans="1:47" ht="24.75" customHeight="1">
+    <row r="19" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>53</v>
       </c>
@@ -2541,7 +2554,7 @@
       <c r="AT19" s="32"/>
       <c r="AU19" s="32"/>
     </row>
-    <row r="20" spans="1:47" ht="24.75" customHeight="1">
+    <row r="20" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>115</v>
       </c>
@@ -2592,7 +2605,7 @@
       <c r="AT20" s="32"/>
       <c r="AU20" s="32"/>
     </row>
-    <row r="21" spans="1:47" ht="24.75" customHeight="1">
+    <row r="21" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>116</v>
       </c>
@@ -2643,7 +2656,7 @@
       <c r="AT21" s="32"/>
       <c r="AU21" s="32"/>
     </row>
-    <row r="22" spans="1:47" ht="24.75" customHeight="1">
+    <row r="22" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>117</v>
       </c>
@@ -2694,7 +2707,7 @@
       <c r="AT22" s="32"/>
       <c r="AU22" s="32"/>
     </row>
-    <row r="23" spans="1:47" ht="24.75" customHeight="1">
+    <row r="23" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>118</v>
       </c>
@@ -2745,7 +2758,7 @@
       <c r="AT23" s="32"/>
       <c r="AU23" s="32"/>
     </row>
-    <row r="24" spans="1:47" ht="24.75" customHeight="1">
+    <row r="24" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>119</v>
       </c>
@@ -2796,7 +2809,7 @@
       <c r="AT24" s="32"/>
       <c r="AU24" s="32"/>
     </row>
-    <row r="25" spans="1:47" ht="24.75" customHeight="1">
+    <row r="25" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>120</v>
       </c>
@@ -2847,7 +2860,7 @@
       <c r="AT25" s="32"/>
       <c r="AU25" s="32"/>
     </row>
-    <row r="26" spans="1:47" ht="24.75" customHeight="1">
+    <row r="26" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>121</v>
       </c>
@@ -2898,7 +2911,7 @@
       <c r="AT26" s="32"/>
       <c r="AU26" s="32"/>
     </row>
-    <row r="27" spans="1:47" ht="24.75" customHeight="1">
+    <row r="27" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>122</v>
       </c>
@@ -2949,7 +2962,7 @@
       <c r="AT27" s="32"/>
       <c r="AU27" s="32"/>
     </row>
-    <row r="28" spans="1:47" ht="24.75" customHeight="1">
+    <row r="28" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>123</v>
       </c>
@@ -3000,7 +3013,7 @@
       <c r="AT28" s="32"/>
       <c r="AU28" s="32"/>
     </row>
-    <row r="29" spans="1:47" ht="24.75" customHeight="1">
+    <row r="29" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>124</v>
       </c>
@@ -3051,7 +3064,7 @@
       <c r="AT29" s="32"/>
       <c r="AU29" s="32"/>
     </row>
-    <row r="30" spans="1:47" ht="24.75" customHeight="1">
+    <row r="30" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>125</v>
       </c>
@@ -3102,7 +3115,7 @@
       <c r="AT30" s="32"/>
       <c r="AU30" s="32"/>
     </row>
-    <row r="31" spans="1:47" ht="24.75" customHeight="1">
+    <row r="31" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>126</v>
       </c>
@@ -3153,7 +3166,7 @@
       <c r="AT31" s="32"/>
       <c r="AU31" s="32"/>
     </row>
-    <row r="32" spans="1:47" ht="24.75" customHeight="1">
+    <row r="32" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>127</v>
       </c>
@@ -3204,7 +3217,7 @@
       <c r="AT32" s="32"/>
       <c r="AU32" s="32"/>
     </row>
-    <row r="33" spans="1:47" ht="24.75" customHeight="1">
+    <row r="33" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>128</v>
       </c>
@@ -3255,7 +3268,7 @@
       <c r="AT33" s="32"/>
       <c r="AU33" s="32"/>
     </row>
-    <row r="34" spans="1:47" ht="24.75" customHeight="1">
+    <row r="34" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>129</v>
       </c>
@@ -3306,7 +3319,7 @@
       <c r="AT34" s="32"/>
       <c r="AU34" s="32"/>
     </row>
-    <row r="35" spans="1:47" ht="24.75" customHeight="1">
+    <row r="35" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>130</v>
       </c>
@@ -3357,7 +3370,7 @@
       <c r="AT35" s="32"/>
       <c r="AU35" s="32"/>
     </row>
-    <row r="36" spans="1:47" ht="24.75" customHeight="1">
+    <row r="36" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>131</v>
       </c>
@@ -3408,7 +3421,7 @@
       <c r="AT36" s="32"/>
       <c r="AU36" s="32"/>
     </row>
-    <row r="37" spans="1:47" ht="24.75" customHeight="1">
+    <row r="37" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>132</v>
       </c>
@@ -3459,7 +3472,7 @@
       <c r="AT37" s="32"/>
       <c r="AU37" s="32"/>
     </row>
-    <row r="38" spans="1:47" ht="24.75" customHeight="1">
+    <row r="38" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>133</v>
       </c>
@@ -3510,7 +3523,7 @@
       <c r="AT38" s="32"/>
       <c r="AU38" s="32"/>
     </row>
-    <row r="39" spans="1:47" ht="24.75" customHeight="1">
+    <row r="39" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>134</v>
       </c>
@@ -3561,7 +3574,7 @@
       <c r="AT39" s="32"/>
       <c r="AU39" s="32"/>
     </row>
-    <row r="40" spans="1:47" ht="24.75" customHeight="1">
+    <row r="40" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>135</v>
       </c>
@@ -3612,7 +3625,7 @@
       <c r="AT40" s="32"/>
       <c r="AU40" s="32"/>
     </row>
-    <row r="41" spans="1:47" ht="24.75" customHeight="1">
+    <row r="41" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>136</v>
       </c>
@@ -3663,7 +3676,7 @@
       <c r="AT41" s="32"/>
       <c r="AU41" s="32"/>
     </row>
-    <row r="42" spans="1:47" ht="24.75" customHeight="1"/>
+    <row r="42" spans="1:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -3672,14 +3685,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.125" customWidth="1"/>
     <col min="2" max="2" width="3.125" style="3" bestFit="1" customWidth="1"/>
@@ -3690,7 +3703,7 @@
     <col min="31" max="31" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C1">
         <v>0</v>
       </c>
@@ -3782,7 +3795,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="3" customFormat="1">
+    <row r="2" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -3875,7 +3888,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3973,7 +3986,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4071,7 +4084,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4169,7 +4182,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4267,7 +4280,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4365,7 +4378,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4463,7 +4476,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4561,7 +4574,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4659,7 +4672,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -4757,7 +4770,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4855,7 +4868,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4953,7 +4966,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -5051,7 +5064,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -5149,7 +5162,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -5247,7 +5260,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -5345,7 +5358,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -5443,7 +5456,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -5541,7 +5554,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -5639,7 +5652,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5737,7 +5750,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5835,7 +5848,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5849,7 +5862,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -5863,7 +5876,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -5877,7 +5890,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>24</v>
       </c>
@@ -5888,7 +5901,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>25</v>
       </c>
@@ -5899,7 +5912,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>26</v>
       </c>
@@ -5910,7 +5923,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>27</v>
       </c>
@@ -5921,97 +5934,97 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>46</v>
       </c>
@@ -6023,14 +6036,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="30" width="4.625" customWidth="1"/>
@@ -6044,7 +6057,7 @@
     <col min="40" max="41" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -6133,7 +6146,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
@@ -6228,7 +6241,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="11">
         <v>100</v>
@@ -6319,7 +6332,7 @@
       </c>
       <c r="AE3" s="6"/>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>0</v>
       </c>
@@ -6414,7 +6427,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>1</v>
       </c>
@@ -6506,7 +6519,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>2</v>
       </c>
@@ -6598,7 +6611,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>3</v>
       </c>
@@ -6690,7 +6703,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>4</v>
       </c>
@@ -6809,7 +6822,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>5</v>
       </c>
@@ -6901,7 +6914,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>6</v>
       </c>
@@ -6996,7 +7009,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>7</v>
       </c>
@@ -7088,7 +7101,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>8</v>
       </c>
@@ -7180,7 +7193,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>9</v>
       </c>
@@ -7275,7 +7288,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>10</v>
       </c>
@@ -7370,7 +7383,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>11</v>
       </c>
@@ -7462,7 +7475,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>12</v>
       </c>
@@ -7590,7 +7603,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>13</v>
       </c>
@@ -7685,7 +7698,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>14</v>
       </c>
@@ -7777,7 +7790,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>15</v>
       </c>
@@ -7869,7 +7882,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>16</v>
       </c>
@@ -7961,7 +7974,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>17</v>
       </c>
@@ -8053,7 +8066,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>18</v>
       </c>
@@ -8145,7 +8158,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>19</v>
       </c>
@@ -8240,7 +8253,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>20</v>
       </c>
@@ -8332,7 +8345,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>21</v>
       </c>
@@ -8424,7 +8437,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>22</v>
       </c>
@@ -8516,7 +8529,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>23</v>
       </c>
@@ -8611,7 +8624,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>24</v>
       </c>
@@ -8703,7 +8716,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>25</v>
       </c>
@@ -8795,7 +8808,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>26</v>
       </c>
@@ -8887,7 +8900,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>27</v>
       </c>
@@ -8982,7 +8995,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>28</v>
       </c>
@@ -9077,7 +9090,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>29</v>
       </c>
@@ -9169,7 +9182,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>30</v>
       </c>
@@ -9261,7 +9274,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>31</v>
       </c>
@@ -9353,7 +9366,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>32</v>
       </c>
@@ -9448,7 +9461,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>33</v>
       </c>
@@ -9540,7 +9553,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>34</v>
       </c>
@@ -9632,7 +9645,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>35</v>
       </c>
@@ -9724,7 +9737,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>36</v>
       </c>
@@ -9816,7 +9829,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>37</v>
       </c>
@@ -9908,12 +9921,12 @@
         <v>600</v>
       </c>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="26">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC46" s="9"/>
       <c r="AD46" s="9"/>
     </row>
@@ -9924,14 +9937,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.375" customWidth="1"/>
     <col min="2" max="29" width="4.625" customWidth="1"/>
@@ -9939,7 +9952,7 @@
     <col min="31" max="31" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -10028,7 +10041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -10121,7 +10134,7 @@
       </c>
       <c r="AE2" s="6"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7">
         <v>100</v>
@@ -10211,7 +10224,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -10303,7 +10316,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -10395,7 +10408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -10487,7 +10500,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -10579,7 +10592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -10613,7 +10626,7 @@
       <c r="AC8" s="8"/>
       <c r="AD8" s="8"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>5</v>
       </c>
@@ -10647,7 +10660,7 @@
       <c r="AC9" s="8"/>
       <c r="AD9" s="8"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>6</v>
       </c>
@@ -10681,7 +10694,7 @@
       <c r="AC10" s="8"/>
       <c r="AD10" s="8"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>7</v>
       </c>
@@ -10715,7 +10728,7 @@
       <c r="AC11" s="8"/>
       <c r="AD11" s="8"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>8</v>
       </c>
@@ -10749,7 +10762,7 @@
       <c r="AC12" s="14"/>
       <c r="AD12" s="8"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>9</v>
       </c>
@@ -10783,7 +10796,7 @@
       <c r="AC13" s="8"/>
       <c r="AD13" s="8"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>10</v>
       </c>
@@ -10817,7 +10830,7 @@
       <c r="AC14" s="8"/>
       <c r="AD14" s="8"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>11</v>
       </c>
@@ -10851,7 +10864,7 @@
       <c r="AC15" s="8"/>
       <c r="AD15" s="8"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>12</v>
       </c>
@@ -10885,7 +10898,7 @@
       <c r="AC16" s="8"/>
       <c r="AD16" s="8"/>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>13</v>
       </c>
@@ -10919,7 +10932,7 @@
       <c r="AC17" s="8"/>
       <c r="AD17" s="8"/>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>14</v>
       </c>
@@ -10953,7 +10966,7 @@
       <c r="AC18" s="8"/>
       <c r="AD18" s="8"/>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>15</v>
       </c>
@@ -10987,7 +11000,7 @@
       <c r="AC19" s="8"/>
       <c r="AD19" s="8"/>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>16</v>
       </c>
@@ -11021,477 +11034,477 @@
       <c r="AC20" s="8"/>
       <c r="AD20" s="8"/>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>99</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>103</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>109</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>110</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>111</v>
       </c>
@@ -11503,16 +11516,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>300</v>
       </c>
@@ -11523,7 +11536,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>301</v>
       </c>
@@ -11534,7 +11547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>302</v>
       </c>
@@ -11545,7 +11558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>303</v>
       </c>
@@ -11556,7 +11569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>304</v>
       </c>
@@ -11573,21 +11586,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -11598,7 +11611,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -11609,7 +11622,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
cambios mínimos en la matriz
</commit_message>
<xml_diff>
--- a/docs/matriz-tokens.xlsx
+++ b/docs/matriz-tokens.xlsx
@@ -1296,11 +1296,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="8240" ySplit="7600" topLeftCell="AH33" activePane="bottomRight"/>
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="8240" ySplit="7600" topLeftCell="AH33"/>
+      <selection activeCell="M4" sqref="M4"/>
+      <selection pane="topRight" activeCell="Z1" sqref="Z1"/>
       <selection pane="bottomLeft" activeCell="F40" sqref="A40:XFD40"/>
-      <selection pane="topRight" activeCell="Z1" sqref="Z1"/>
       <selection pane="bottomRight" activeCell="AJ37" sqref="AJ37"/>
     </sheetView>
   </sheetViews>
@@ -1838,7 +1838,7 @@
         <v>103</v>
       </c>
       <c r="C4" s="31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -1893,7 +1893,9 @@
       <c r="B5" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="31"/>
+      <c r="C5" s="31">
+        <v>4</v>
+      </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>

</xml_diff>